<commit_message>
last post compo fixes, compo version
</commit_message>
<xml_diff>
--- a/assetcreation/Balance.xlsx
+++ b/assetcreation/Balance.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:AD23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,7 @@
         <v>10</v>
       </c>
       <c r="Q9">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="U9">
         <v>10</v>

</xml_diff>